<commit_message>
nb elements peut varier (sauf C5)
</commit_message>
<xml_diff>
--- a/data/concentration_corrigeelin.xlsx
+++ b/data/concentration_corrigeelin.xlsx
@@ -1144,211 +1144,211 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11.54758687145696</v>
+        <v>9.768561456389049</v>
       </c>
       <c r="C3" t="n">
-        <v>7003.944438264014</v>
+        <v>5924.91422181299</v>
       </c>
       <c r="D3" t="n">
-        <v>22003.1637508317</v>
+        <v>18613.34837551843</v>
       </c>
       <c r="E3" t="n">
-        <v>22129.17162060167</v>
+        <v>18719.94342724124</v>
       </c>
       <c r="F3" t="n">
-        <v>22173.10128134911</v>
+        <v>18757.10526854598</v>
       </c>
       <c r="G3" t="n">
-        <v>23034.59512676832</v>
+        <v>19485.87706017283</v>
       </c>
       <c r="H3" t="n">
-        <v>22179.52782785283</v>
+        <v>18762.54173896813</v>
       </c>
       <c r="I3" t="n">
-        <v>24920.10557726619</v>
+        <v>21080.90508787957</v>
       </c>
       <c r="J3" t="n">
-        <v>25556.08044864375</v>
+        <v>21618.90144027133</v>
       </c>
       <c r="K3" t="n">
-        <v>22829.33475198876</v>
+        <v>19312.23917306139</v>
       </c>
       <c r="L3" t="n">
-        <v>23792.47364864461</v>
+        <v>20126.99654252333</v>
       </c>
       <c r="M3" t="n">
-        <v>22747.89888879649</v>
+        <v>19243.34934844235</v>
       </c>
       <c r="N3" t="n">
-        <v>24034.576262631</v>
+        <v>20331.80074012795</v>
       </c>
       <c r="O3" t="n">
-        <v>22202.55345530682</v>
+        <v>18782.02002991843</v>
       </c>
       <c r="P3" t="n">
-        <v>24688.23108534628</v>
+        <v>20884.75326415202</v>
       </c>
       <c r="Q3" t="n">
-        <v>25271.92271198188</v>
+        <v>21378.52114741975</v>
       </c>
       <c r="R3" t="n">
-        <v>25254.46511112387</v>
+        <v>21363.75307087173</v>
       </c>
       <c r="S3" t="n">
-        <v>25400.07070511902</v>
+        <v>21486.9266143288</v>
       </c>
       <c r="T3" t="n">
-        <v>25160.82776535774</v>
+        <v>21284.5415285026</v>
       </c>
       <c r="U3" t="n">
-        <v>25957.31188927296</v>
+        <v>21958.31901986191</v>
       </c>
       <c r="V3" t="n">
-        <v>21908.90311892793</v>
+        <v>18867.81724346393</v>
       </c>
       <c r="W3" t="n">
-        <v>22754.63001075225</v>
+        <v>19596.15221971557</v>
       </c>
       <c r="X3" t="n">
-        <v>22353.10496894401</v>
+        <v>19250.36123846982</v>
       </c>
       <c r="Y3" t="n">
-        <v>22552.52733308657</v>
+        <v>19422.10259404917</v>
       </c>
       <c r="Z3" t="n">
-        <v>21794.11004139778</v>
+        <v>18768.95812688029</v>
       </c>
       <c r="AA3" t="n">
-        <v>20411.26767410164</v>
+        <v>17578.06249321794</v>
       </c>
       <c r="AB3" t="n">
-        <v>21340.21331555299</v>
+        <v>18378.06496239104</v>
       </c>
       <c r="AC3" t="n">
-        <v>22629.78429125573</v>
+        <v>19488.6358275757</v>
       </c>
       <c r="AD3" t="n">
-        <v>22205.16573851251</v>
+        <v>19122.956851871</v>
       </c>
       <c r="AE3" t="n">
-        <v>23217.29787198834</v>
+        <v>19994.5990339098</v>
       </c>
       <c r="AF3" t="n">
-        <v>22782.01378282982</v>
+        <v>19619.73496158958</v>
       </c>
       <c r="AG3" t="n">
-        <v>22234.87797924066</v>
+        <v>19689.51951023078</v>
       </c>
       <c r="AH3" t="n">
-        <v>17102.32632031897</v>
+        <v>15144.52150664574</v>
       </c>
       <c r="AI3" t="n">
-        <v>20925.28912581072</v>
+        <v>18529.84706660129</v>
       </c>
       <c r="AJ3" t="n">
-        <v>20603.80493898815</v>
+        <v>18245.16508298153</v>
       </c>
       <c r="AK3" t="n">
-        <v>22526.00119208144</v>
+        <v>19947.31612078387</v>
       </c>
       <c r="AL3" t="n">
-        <v>23043.96446589386</v>
+        <v>20405.98506400156</v>
       </c>
       <c r="AM3" t="n">
-        <v>23170.80818227932</v>
+        <v>20518.30822722528</v>
       </c>
       <c r="AN3" t="n">
-        <v>23453.60406869433</v>
+        <v>20768.73078983974</v>
       </c>
       <c r="AO3" t="n">
-        <v>24262.92856396277</v>
+        <v>21485.40710596675</v>
       </c>
       <c r="AP3" t="n">
-        <v>22913.72615163351</v>
+        <v>20290.6559026721</v>
       </c>
       <c r="AQ3" t="n">
-        <v>42388.95365004531</v>
+        <v>37536.43850396064</v>
       </c>
       <c r="AR3" t="n">
-        <v>16.11955178479527</v>
+        <v>14.60015565294584</v>
       </c>
       <c r="AS3" t="n">
-        <v>6722.28175730044</v>
+        <v>6088.653165413758</v>
       </c>
       <c r="AT3" t="n">
-        <v>18155.32763337259</v>
+        <v>16444.0434148731</v>
       </c>
       <c r="AU3" t="n">
-        <v>19799.14687768607</v>
+        <v>17932.91960403133</v>
       </c>
       <c r="AV3" t="n">
-        <v>18116.57090568549</v>
+        <v>16408.93981742915</v>
       </c>
       <c r="AW3" t="n">
-        <v>22687.64169840196</v>
+        <v>20549.15078391804</v>
       </c>
       <c r="AX3" t="n">
-        <v>20429.73917291164</v>
+        <v>18504.07355339398</v>
       </c>
       <c r="AY3" t="n">
-        <v>22768.26915488419</v>
+        <v>20622.17846050964</v>
       </c>
       <c r="AZ3" t="n">
-        <v>22916.94361650572</v>
+        <v>20756.83917007972</v>
       </c>
       <c r="BA3" t="n">
-        <v>23959.09033065243</v>
+        <v>21700.75525676025</v>
       </c>
       <c r="BB3" t="n">
-        <v>18452.66807159899</v>
+        <v>16713.35714877701</v>
       </c>
       <c r="BC3" t="n">
-        <v>22724.42707388896</v>
+        <v>20582.46884480661</v>
       </c>
       <c r="BD3" t="n">
-        <v>22715.16143571463</v>
+        <v>20574.07656682176</v>
       </c>
       <c r="BE3" t="n">
-        <v>19049.47611762205</v>
+        <v>18455.12502136194</v>
       </c>
       <c r="BF3" t="n">
-        <v>19949.28167893385</v>
+        <v>19326.85629766535</v>
       </c>
       <c r="BG3" t="n">
-        <v>19416.23876153472</v>
+        <v>18810.44452751424</v>
       </c>
       <c r="BH3" t="n">
-        <v>20100.73659395595</v>
+        <v>19473.58576017518</v>
       </c>
       <c r="BI3" t="n">
-        <v>21157.26125635687</v>
+        <v>20497.14644039378</v>
       </c>
       <c r="BJ3" t="n">
-        <v>20304.05003861152</v>
+        <v>19670.55574593617</v>
       </c>
       <c r="BK3" t="n">
-        <v>19931.98794614142</v>
+        <v>19310.10213609157</v>
       </c>
       <c r="BL3" t="n">
-        <v>20923.54146997829</v>
+        <v>20270.71880264931</v>
       </c>
       <c r="BM3" t="n">
-        <v>834.6021940609628</v>
+        <v>808.5622795815112</v>
       </c>
       <c r="BN3" t="n">
-        <v>848.3711890628722</v>
+        <v>821.9016765607109</v>
       </c>
       <c r="BO3" t="n">
-        <v>706.1701590217508</v>
+        <v>684.1373742055587</v>
       </c>
       <c r="BP3" t="n">
-        <v>812.6135125465538</v>
+        <v>787.2596535198984</v>
       </c>
       <c r="BQ3" t="n">
-        <v>14.63550741258335</v>
+        <v>14.06231283692968</v>
       </c>
       <c r="BR3" t="n">
-        <v>6252.966212753088</v>
+        <v>6008.070958092214</v>
       </c>
     </row>
     <row r="4">
@@ -1358,211 +1358,211 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>18.84644252316956</v>
+        <v>16.56963241710433</v>
       </c>
       <c r="C4" t="n">
-        <v>3380.61854469357</v>
+        <v>2972.211151210834</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2783582282610468</v>
+        <v>0.2447301933450663</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4216293503836486</v>
+        <v>0.3706929487371821</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3847941467155964</v>
+        <v>0.3383077500961947</v>
       </c>
       <c r="G4" t="n">
-        <v>0.493178180292253</v>
+        <v>0.433598073139414</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9756283841586556</v>
+        <v>0.8577642003963535</v>
       </c>
       <c r="I4" t="n">
-        <v>0.7614935392169196</v>
+        <v>0.6694986609442172</v>
       </c>
       <c r="J4" t="n">
-        <v>0.8377852058469887</v>
+        <v>0.736573647164795</v>
       </c>
       <c r="K4" t="n">
-        <v>0.517126561017467</v>
+        <v>0.4546532863508104</v>
       </c>
       <c r="L4" t="n">
-        <v>0.3786245020126358</v>
+        <v>0.332883450802229</v>
       </c>
       <c r="M4" t="n">
-        <v>0.4699719605712805</v>
+        <v>0.4131953615881837</v>
       </c>
       <c r="N4" t="n">
-        <v>1.003373150777234</v>
+        <v>0.8821571638855118</v>
       </c>
       <c r="O4" t="n">
-        <v>1.008618890150674</v>
+        <v>0.8867691734500209</v>
       </c>
       <c r="P4" t="n">
-        <v>0.8683757665208893</v>
+        <v>0.7634686086503123</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.8528911500070974</v>
+        <v>0.749854665146761</v>
       </c>
       <c r="R4" t="n">
-        <v>0.4704320727871774</v>
+        <v>0.4135998883458812</v>
       </c>
       <c r="S4" t="n">
-        <v>0.7254768751809478</v>
+        <v>0.6378331154051736</v>
       </c>
       <c r="T4" t="n">
-        <v>0.3844278973917425</v>
+        <v>0.3379857467970674</v>
       </c>
       <c r="U4" t="n">
-        <v>0.181418105718176</v>
+        <v>0.1595012598192988</v>
       </c>
       <c r="V4" t="n">
-        <v>0.1424478757363488</v>
+        <v>0.1269360380684472</v>
       </c>
       <c r="W4" t="n">
-        <v>0.172412711283359</v>
+        <v>0.1536378578467219</v>
       </c>
       <c r="X4" t="n">
-        <v>0.0570274264647896</v>
+        <v>0.05081743437212209</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.1993133631490336</v>
+        <v>0.1776091677145319</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.01615636677791429</v>
+        <v>0.01439702191252692</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.03694130958957266</v>
+        <v>0.03291859184365315</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.1331034249884807</v>
+        <v>0.1186091497261071</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.162537048065379</v>
+        <v>0.1448376033275961</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.2767983623740568</v>
+        <v>0.2466564508734998</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.2661413759666764</v>
+        <v>0.2371599552233581</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.5222464591434738</v>
+        <v>0.4653765180861303</v>
       </c>
       <c r="AG4" t="n">
-        <v>-0.02332373019058488</v>
+        <v>-0.02063148376841588</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.500578097580515</v>
+        <v>0.4427966200374705</v>
       </c>
       <c r="AI4" t="n">
-        <v>3.171448544512217</v>
+        <v>2.80536983723482</v>
       </c>
       <c r="AJ4" t="n">
-        <v>6.448070799620875</v>
+        <v>5.703773236653036</v>
       </c>
       <c r="AK4" t="n">
-        <v>0.7550456619218172</v>
+        <v>0.6678911216629091</v>
       </c>
       <c r="AL4" t="n">
-        <v>3.428102196160052</v>
+        <v>3.032398087210652</v>
       </c>
       <c r="AM4" t="n">
-        <v>2.636598110822769</v>
+        <v>2.332256919574314</v>
       </c>
       <c r="AN4" t="n">
-        <v>5.359126337026309</v>
+        <v>4.740525084614506</v>
       </c>
       <c r="AO4" t="n">
-        <v>7.035908036671416</v>
+        <v>6.223756717664765</v>
       </c>
       <c r="AP4" t="n">
-        <v>8.460724672486066</v>
+        <v>7.484107487227569</v>
       </c>
       <c r="AQ4" t="n">
-        <v>19.616820543762</v>
+        <v>17.35246083407053</v>
       </c>
       <c r="AR4" t="n">
-        <v>17.37313771761699</v>
+        <v>16.43590608149136</v>
       </c>
       <c r="AS4" t="n">
-        <v>3175.666620574099</v>
+        <v>3004.348389465385</v>
       </c>
       <c r="AT4" t="n">
-        <v>3.438017415595697</v>
+        <v>3.252546101212474</v>
       </c>
       <c r="AU4" t="n">
-        <v>3.042542463708205</v>
+        <v>2.878405904291459</v>
       </c>
       <c r="AV4" t="n">
-        <v>3.51134197813409</v>
+        <v>3.321915011016567</v>
       </c>
       <c r="AW4" t="n">
-        <v>2.557412671383349</v>
+        <v>2.419447491966248</v>
       </c>
       <c r="AX4" t="n">
-        <v>1.019611739394812</v>
+        <v>0.9646065702504453</v>
       </c>
       <c r="AY4" t="n">
-        <v>1.1035638627986</v>
+        <v>1.044029714073639</v>
       </c>
       <c r="AZ4" t="n">
-        <v>0.807475387794503</v>
+        <v>0.7639143747446607</v>
       </c>
       <c r="BA4" t="n">
-        <v>0.7216955785752071</v>
+        <v>0.6827621435856952</v>
       </c>
       <c r="BB4" t="n">
-        <v>4.072802001320003</v>
+        <v>3.853085854164722</v>
       </c>
       <c r="BC4" t="n">
-        <v>0.7324997946555269</v>
+        <v>0.6929835027705826</v>
       </c>
       <c r="BD4" t="n">
-        <v>1.178410442821188</v>
+        <v>1.114838532824015</v>
       </c>
       <c r="BE4" t="n">
-        <v>1.027178592903335</v>
+        <v>0.994971917106736</v>
       </c>
       <c r="BF4" t="n">
-        <v>1.402929430104518</v>
+        <v>1.358941272998196</v>
       </c>
       <c r="BG4" t="n">
-        <v>1.268579372789026</v>
+        <v>1.228803695157168</v>
       </c>
       <c r="BH4" t="n">
-        <v>1.813073814658782</v>
+        <v>1.756225783608048</v>
       </c>
       <c r="BI4" t="n">
-        <v>1.960024273886376</v>
+        <v>1.89856868400293</v>
       </c>
       <c r="BJ4" t="n">
-        <v>2.488998322470729</v>
+        <v>2.410957013409261</v>
       </c>
       <c r="BK4" t="n">
-        <v>2.623939029886982</v>
+        <v>2.541666721809817</v>
       </c>
       <c r="BL4" t="n">
-        <v>1.017619998938912</v>
+        <v>0.9857130281196268</v>
       </c>
       <c r="BM4" t="n">
-        <v>-0.01740253950200887</v>
+        <v>-0.01685689149916791</v>
       </c>
       <c r="BN4" t="n">
-        <v>0.07385971317667388</v>
+        <v>0.0715438784687218</v>
       </c>
       <c r="BO4" t="n">
-        <v>0.04763589055515458</v>
+        <v>0.04614229081116487</v>
       </c>
       <c r="BP4" t="n">
-        <v>-0.1373541982960943</v>
+        <v>-0.1330475254697844</v>
       </c>
       <c r="BQ4" t="n">
-        <v>17.32111362698448</v>
+        <v>16.97999846527934</v>
       </c>
       <c r="BR4" t="n">
-        <v>3132.641735950009</v>
+        <v>3070.948728483208</v>
       </c>
     </row>
     <row r="5">
@@ -1572,211 +1572,211 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>30.32625000889527</v>
+        <v>27.34272202821066</v>
       </c>
       <c r="C5" t="n">
-        <v>13164.60222149426</v>
+        <v>11869.45497872965</v>
       </c>
       <c r="D5" t="n">
-        <v>7.329638947246216</v>
+        <v>6.60854145312774</v>
       </c>
       <c r="E5" t="n">
-        <v>8.508204306271494</v>
+        <v>7.671158327764538</v>
       </c>
       <c r="F5" t="n">
-        <v>12.1730956348732</v>
+        <v>10.97549384013957</v>
       </c>
       <c r="G5" t="n">
-        <v>32.79834869270857</v>
+        <v>29.57161307533933</v>
       </c>
       <c r="H5" t="n">
-        <v>55.15042059630027</v>
+        <v>49.72466492432225</v>
       </c>
       <c r="I5" t="n">
-        <v>78.46793599238457</v>
+        <v>70.74817893204315</v>
       </c>
       <c r="J5" t="n">
-        <v>84.65005093136146</v>
+        <v>76.32209098095497</v>
       </c>
       <c r="K5" t="n">
-        <v>12.47488654500039</v>
+        <v>11.24759424700913</v>
       </c>
       <c r="L5" t="n">
-        <v>18.25274537436404</v>
+        <v>16.45702132233805</v>
       </c>
       <c r="M5" t="n">
-        <v>16.18303457072033</v>
+        <v>14.59093081770213</v>
       </c>
       <c r="N5" t="n">
-        <v>37.36918759152066</v>
+        <v>33.69276809481232</v>
       </c>
       <c r="O5" t="n">
-        <v>53.84222885587751</v>
+        <v>48.54517444635387</v>
       </c>
       <c r="P5" t="n">
-        <v>76.2108274045476</v>
+        <v>68.71312703190345</v>
       </c>
       <c r="Q5" t="n">
-        <v>84.04589427127826</v>
+        <v>75.77737188072656</v>
       </c>
       <c r="R5" t="n">
-        <v>21.47213583563514</v>
+        <v>19.35968480552468</v>
       </c>
       <c r="S5" t="n">
-        <v>41.36518666151905</v>
+        <v>37.29563662500995</v>
       </c>
       <c r="T5" t="n">
-        <v>5.274442849280056</v>
+        <v>4.755537682346026</v>
       </c>
       <c r="U5" t="n">
-        <v>4.498409080381567</v>
+        <v>4.055850921824296</v>
       </c>
       <c r="V5" t="n">
-        <v>4.993978162322223</v>
+        <v>4.565756708143097</v>
       </c>
       <c r="W5" t="n">
-        <v>9.355283040293173</v>
+        <v>8.553090323873928</v>
       </c>
       <c r="X5" t="n">
-        <v>5.461707922442754</v>
+        <v>4.993379781463755</v>
       </c>
       <c r="Y5" t="n">
-        <v>7.580386168212258</v>
+        <v>6.930386532114182</v>
       </c>
       <c r="Z5" t="n">
-        <v>7.19519695399535</v>
+        <v>6.578226354085406</v>
       </c>
       <c r="AA5" t="n">
-        <v>10.62090474414873</v>
+        <v>9.710188051682767</v>
       </c>
       <c r="AB5" t="n">
-        <v>15.45007694981672</v>
+        <v>14.12527051222641</v>
       </c>
       <c r="AC5" t="n">
-        <v>16.41318755293549</v>
+        <v>15.00579672879051</v>
       </c>
       <c r="AD5" t="n">
-        <v>7.002602346886895</v>
+        <v>6.402146265071017</v>
       </c>
       <c r="AE5" t="n">
-        <v>8.777361651391303</v>
+        <v>8.024724285338609</v>
       </c>
       <c r="AF5" t="n">
-        <v>30.90139200782199</v>
+        <v>28.2516729678822</v>
       </c>
       <c r="AG5" t="n">
-        <v>3.386853187904942</v>
+        <v>3.148974908402798</v>
       </c>
       <c r="AH5" t="n">
-        <v>5.018647033872989</v>
+        <v>4.66615843882269</v>
       </c>
       <c r="AI5" t="n">
-        <v>16.57845508074922</v>
+        <v>15.41405433686824</v>
       </c>
       <c r="AJ5" t="n">
-        <v>25.13574051280247</v>
+        <v>23.37031214154896</v>
       </c>
       <c r="AK5" t="n">
-        <v>7.596527556353893</v>
+        <v>7.062979508936492</v>
       </c>
       <c r="AL5" t="n">
-        <v>62.618323496131</v>
+        <v>58.2202766272077</v>
       </c>
       <c r="AM5" t="n">
-        <v>15.78305670242298</v>
+        <v>14.67452138501833</v>
       </c>
       <c r="AN5" t="n">
-        <v>28.56413924606734</v>
+        <v>26.55791461147746</v>
       </c>
       <c r="AO5" t="n">
-        <v>25.84873337046434</v>
+        <v>24.03322738885453</v>
       </c>
       <c r="AP5" t="n">
-        <v>25.94485029223761</v>
+        <v>24.12259346353937</v>
       </c>
       <c r="AQ5" t="n">
-        <v>71.71213605357484</v>
+        <v>66.67537815548587</v>
       </c>
       <c r="AR5" t="n">
-        <v>28.72911573865936</v>
+        <v>26.92474471995898</v>
       </c>
       <c r="AS5" t="n">
-        <v>12850.876896131</v>
+        <v>12043.76017011697</v>
       </c>
       <c r="AT5" t="n">
-        <v>101.3692872959033</v>
+        <v>95.00265193382326</v>
       </c>
       <c r="AU5" t="n">
-        <v>344.2628628601309</v>
+        <v>322.6409675602434</v>
       </c>
       <c r="AV5" t="n">
-        <v>505.7550939505013</v>
+        <v>473.9904603855229</v>
       </c>
       <c r="AW5" t="n">
-        <v>43.43246877597446</v>
+        <v>40.70463375860493</v>
       </c>
       <c r="AX5" t="n">
-        <v>321.3617385173264</v>
+        <v>301.1781793443043</v>
       </c>
       <c r="AY5" t="n">
-        <v>429.1966481071599</v>
+        <v>402.2403714081946</v>
       </c>
       <c r="AZ5" t="n">
-        <v>565.0378310210053</v>
+        <v>529.5498648741157</v>
       </c>
       <c r="BA5" t="n">
-        <v>616.2707260958454</v>
+        <v>577.5650085946122</v>
       </c>
       <c r="BB5" t="n">
-        <v>22.94584715740283</v>
+        <v>21.50470215360335</v>
       </c>
       <c r="BC5" t="n">
-        <v>12.59741127060698</v>
+        <v>11.80621379644506</v>
       </c>
       <c r="BD5" t="n">
-        <v>9.090639805222118</v>
+        <v>8.519689861784972</v>
       </c>
       <c r="BE5" t="n">
-        <v>8.550220780411731</v>
+        <v>8.070889798485169</v>
       </c>
       <c r="BF5" t="n">
-        <v>5.062846537779635</v>
+        <v>4.779020041994043</v>
       </c>
       <c r="BG5" t="n">
-        <v>5.062846537779633</v>
+        <v>4.779020041994042</v>
       </c>
       <c r="BH5" t="n">
-        <v>4.597914964492386</v>
+        <v>4.340152837484616</v>
       </c>
       <c r="BI5" t="n">
-        <v>4.856210282985301</v>
+        <v>4.583967951100964</v>
       </c>
       <c r="BJ5" t="n">
-        <v>18.65073006241795</v>
+        <v>17.60515790889567</v>
       </c>
       <c r="BK5" t="n">
-        <v>8.976408055925042</v>
+        <v>8.473184735952143</v>
       </c>
       <c r="BL5" t="n">
-        <v>67.94626244913158</v>
+        <v>64.13715043501892</v>
       </c>
       <c r="BM5" t="n">
-        <v>698.5998537861153</v>
+        <v>659.4358880255813</v>
       </c>
       <c r="BN5" t="n">
-        <v>489.7254700570419</v>
+        <v>462.271139173017</v>
       </c>
       <c r="BO5" t="n">
-        <v>495.4984995730178</v>
+        <v>467.7205288698992</v>
       </c>
       <c r="BP5" t="n">
-        <v>583.9171198182388</v>
+        <v>551.1823433025933</v>
       </c>
       <c r="BQ5" t="n">
-        <v>28.62193756830286</v>
+        <v>27.27118823258198</v>
       </c>
       <c r="BR5" t="n">
-        <v>12626.81014413733</v>
+        <v>12030.91563581601</v>
       </c>
     </row>
     <row r="6">
@@ -1786,211 +1786,211 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>25.5626317444182</v>
+        <v>23.1463985036059</v>
       </c>
       <c r="C6" t="n">
-        <v>12709.37123263681</v>
+        <v>11508.05496954014</v>
       </c>
       <c r="D6" t="n">
-        <v>8.268386561324951</v>
+        <v>7.486841427118591</v>
       </c>
       <c r="E6" t="n">
-        <v>9.782080115205501</v>
+        <v>8.85745751081307</v>
       </c>
       <c r="F6" t="n">
-        <v>13.12816244377452</v>
+        <v>11.88726116238129</v>
       </c>
       <c r="G6" t="n">
-        <v>33.81240479392731</v>
+        <v>30.61638580684755</v>
       </c>
       <c r="H6" t="n">
-        <v>54.37059361469434</v>
+        <v>49.23137176429908</v>
       </c>
       <c r="I6" t="n">
-        <v>78.51860752318845</v>
+        <v>71.09686505877066</v>
       </c>
       <c r="J6" t="n">
-        <v>84.56845196732417</v>
+        <v>76.57486559443025</v>
       </c>
       <c r="K6" t="n">
-        <v>10.95249302590405</v>
+        <v>9.917240553328222</v>
       </c>
       <c r="L6" t="n">
-        <v>15.26873442675562</v>
+        <v>13.82550181925549</v>
       </c>
       <c r="M6" t="n">
-        <v>13.16283396091541</v>
+        <v>11.91865545544515</v>
       </c>
       <c r="N6" t="n">
-        <v>36.98052600027651</v>
+        <v>33.48504959244918</v>
       </c>
       <c r="O6" t="n">
-        <v>53.67063857445311</v>
+        <v>48.59757793360053</v>
       </c>
       <c r="P6" t="n">
-        <v>79.0858937158231</v>
+        <v>71.61053017790231</v>
       </c>
       <c r="Q6" t="n">
-        <v>85.41077228050932</v>
+        <v>77.33756803569679</v>
       </c>
       <c r="R6" t="n">
-        <v>20.82562891848324</v>
+        <v>18.85714705962108</v>
       </c>
       <c r="S6" t="n">
-        <v>39.50400710120626</v>
+        <v>35.77000599922417</v>
       </c>
       <c r="T6" t="n">
-        <v>2.31846060856287</v>
+        <v>2.099314878736099</v>
       </c>
       <c r="U6" t="n">
-        <v>1.175043633453119</v>
+        <v>1.06397605970167</v>
       </c>
       <c r="V6" t="n">
-        <v>5.478988047666301</v>
+        <v>5.024337112686712</v>
       </c>
       <c r="W6" t="n">
-        <v>9.242449467454648</v>
+        <v>8.475503408196554</v>
       </c>
       <c r="X6" t="n">
-        <v>6.467793317528757</v>
+        <v>5.931090507906513</v>
       </c>
       <c r="Y6" t="n">
-        <v>7.183254505498835</v>
+        <v>6.587182137990668</v>
       </c>
       <c r="Z6" t="n">
-        <v>8.191160615959806</v>
+        <v>7.511451370344576</v>
       </c>
       <c r="AA6" t="n">
-        <v>11.48973417168751</v>
+        <v>10.53630657915065</v>
       </c>
       <c r="AB6" t="n">
-        <v>17.37161870246657</v>
+        <v>15.93010749337579</v>
       </c>
       <c r="AC6" t="n">
-        <v>18.90146478089161</v>
+        <v>17.33300568582633</v>
       </c>
       <c r="AD6" t="n">
-        <v>9.631003049919068</v>
+        <v>8.831814494780303</v>
       </c>
       <c r="AE6" t="n">
-        <v>8.579653752726133</v>
+        <v>7.867707027063982</v>
       </c>
       <c r="AF6" t="n">
-        <v>30.02916376137962</v>
+        <v>27.53731905173809</v>
       </c>
       <c r="AG6" t="n">
-        <v>3.844220337070399</v>
+        <v>3.582030443499851</v>
       </c>
       <c r="AH6" t="n">
-        <v>5.27870626627499</v>
+        <v>4.918679183332196</v>
       </c>
       <c r="AI6" t="n">
-        <v>17.52648939005266</v>
+        <v>16.33111868158146</v>
       </c>
       <c r="AJ6" t="n">
-        <v>26.73230095170512</v>
+        <v>24.90906020927546</v>
       </c>
       <c r="AK6" t="n">
-        <v>9.958842831053664</v>
+        <v>9.27961330906699</v>
       </c>
       <c r="AL6" t="n">
-        <v>65.86726733092176</v>
+        <v>61.37487868068168</v>
       </c>
       <c r="AM6" t="n">
-        <v>17.31297883651868</v>
+        <v>16.13217032906583</v>
       </c>
       <c r="AN6" t="n">
-        <v>30.92516532141823</v>
+        <v>28.81595588665067</v>
       </c>
       <c r="AO6" t="n">
-        <v>28.12935856502237</v>
+        <v>26.21083338131984</v>
       </c>
       <c r="AP6" t="n">
-        <v>28.26139233730951</v>
+        <v>26.3338619672055</v>
       </c>
       <c r="AQ6" t="n">
-        <v>72.99983011053844</v>
+        <v>68.02097457960491</v>
       </c>
       <c r="AR6" t="n">
-        <v>22.73297686656489</v>
+        <v>21.3789269916168</v>
       </c>
       <c r="AS6" t="n">
-        <v>12308.02226008589</v>
+        <v>11574.91651243349</v>
       </c>
       <c r="AT6" t="n">
-        <v>101.0657003766681</v>
+        <v>95.04589928507232</v>
       </c>
       <c r="AU6" t="n">
-        <v>349.8503304547027</v>
+        <v>329.0121094428533</v>
       </c>
       <c r="AV6" t="n">
-        <v>510.8748941973648</v>
+        <v>480.4455276140789</v>
       </c>
       <c r="AW6" t="n">
-        <v>46.45556058697517</v>
+        <v>43.68851664140404</v>
       </c>
       <c r="AX6" t="n">
-        <v>327.686268248686</v>
+        <v>308.1682107083677</v>
       </c>
       <c r="AY6" t="n">
-        <v>435.0390245195655</v>
+        <v>409.1266884359162</v>
       </c>
       <c r="AZ6" t="n">
-        <v>573.8628776439785</v>
+        <v>539.6817423587871</v>
       </c>
       <c r="BA6" t="n">
-        <v>624.315691356528</v>
+        <v>587.1294227577697</v>
       </c>
       <c r="BB6" t="n">
-        <v>25.0352450815396</v>
+        <v>23.54406464041527</v>
       </c>
       <c r="BC6" t="n">
-        <v>13.1225664963823</v>
+        <v>12.34094385066721</v>
       </c>
       <c r="BD6" t="n">
-        <v>9.91086917840533</v>
+        <v>9.320545647509375</v>
       </c>
       <c r="BE6" t="n">
-        <v>7.094207485888878</v>
+        <v>6.725162596282973</v>
       </c>
       <c r="BF6" t="n">
-        <v>5.474403046272593</v>
+        <v>5.1896213462887</v>
       </c>
       <c r="BG6" t="n">
-        <v>5.582496085948486</v>
+        <v>5.292091321799396</v>
       </c>
       <c r="BH6" t="n">
-        <v>4.833638223019265</v>
+        <v>4.582189489956797</v>
       </c>
       <c r="BI6" t="n">
-        <v>5.512598896942893</v>
+        <v>5.225830226106784</v>
       </c>
       <c r="BJ6" t="n">
-        <v>18.59413789518336</v>
+        <v>17.62685979111123</v>
       </c>
       <c r="BK6" t="n">
-        <v>9.794406524996432</v>
+        <v>9.284895676608864</v>
       </c>
       <c r="BL6" t="n">
-        <v>69.30940316670876</v>
+        <v>65.70388682239727</v>
       </c>
       <c r="BM6" t="n">
-        <v>720.6170118376781</v>
+        <v>683.1300866087844</v>
       </c>
       <c r="BN6" t="n">
-        <v>496.8979476285134</v>
+        <v>471.0490210792514</v>
       </c>
       <c r="BO6" t="n">
-        <v>502.6635321353264</v>
+        <v>476.5146764534499</v>
       </c>
       <c r="BP6" t="n">
-        <v>587.3592793102872</v>
+        <v>556.8045005244634</v>
       </c>
       <c r="BQ6" t="n">
-        <v>22.98572601993059</v>
+        <v>21.86227769667273</v>
       </c>
       <c r="BR6" t="n">
-        <v>12140.99445857075</v>
+        <v>11547.59228126569</v>
       </c>
     </row>
     <row r="7">
@@ -2000,211 +2000,211 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>15.98853906016267</v>
+        <v>15.61640032865245</v>
       </c>
       <c r="C7" t="n">
-        <v>63.10737019626775</v>
+        <v>61.63852450590071</v>
       </c>
       <c r="D7" t="n">
-        <v>0.02217161959229226</v>
+        <v>0.02165556754028453</v>
       </c>
       <c r="E7" t="n">
-        <v>0.02773135106233686</v>
+        <v>0.02708589435309218</v>
       </c>
       <c r="F7" t="n">
-        <v>0.04713064786566303</v>
+        <v>0.04603366586837201</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1603169465834623</v>
+        <v>0.1565855146548371</v>
       </c>
       <c r="H7" t="n">
-        <v>0.2292458796563938</v>
+        <v>0.2239101031643541</v>
       </c>
       <c r="I7" t="n">
-        <v>0.3457109561126473</v>
+        <v>0.3376644150126228</v>
       </c>
       <c r="J7" t="n">
-        <v>0.4320257996185174</v>
+        <v>0.4219702509254972</v>
       </c>
       <c r="K7" t="n">
-        <v>0.02861561643077226</v>
+        <v>0.0279495781417291</v>
       </c>
       <c r="L7" t="n">
-        <v>0.02709028353707633</v>
+        <v>0.02645974789440098</v>
       </c>
       <c r="M7" t="n">
-        <v>0.0579528689974274</v>
+        <v>0.05660399609072036</v>
       </c>
       <c r="N7" t="n">
-        <v>0.1656364642329476</v>
+        <v>0.1617812187061647</v>
       </c>
       <c r="O7" t="n">
-        <v>0.2286485777961628</v>
+        <v>0.223326703709825</v>
       </c>
       <c r="P7" t="n">
-        <v>0.3486880160088534</v>
+        <v>0.3405721828184612</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.4323024848266011</v>
+        <v>0.4222404961904455</v>
       </c>
       <c r="R7" t="n">
-        <v>0.0546253522229176</v>
+        <v>0.05335392841064537</v>
       </c>
       <c r="S7" t="n">
-        <v>0.1436956090562651</v>
+        <v>0.1403510444605525</v>
       </c>
       <c r="T7" t="n">
-        <v>0.007692478745057988</v>
+        <v>0.007513433663353939</v>
       </c>
       <c r="U7" t="n">
-        <v>0.00390144379091838</v>
+        <v>0.00381063634829041</v>
       </c>
       <c r="V7" t="n">
-        <v>0.01049454519543809</v>
+        <v>0.01022368524251513</v>
       </c>
       <c r="W7" t="n">
-        <v>0.01383049855088823</v>
+        <v>0.01347353899555437</v>
       </c>
       <c r="X7" t="n">
-        <v>0.005930283712300303</v>
+        <v>0.005777225496129895</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.004903066763928907</v>
+        <v>0.004776520600362598</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.009742597610222347</v>
+        <v>0.009491145119341723</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.02423021638925538</v>
+        <v>0.02360484433660465</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.03937527307602139</v>
+        <v>0.03835901325598307</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.04551840211240051</v>
+        <v>0.0443435906247476</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.004977244947768313</v>
+        <v>0.004848784275377803</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.01002850923958194</v>
+        <v>0.009769677485567351</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.01360796399937001</v>
+        <v>0.01325674797050876</v>
       </c>
       <c r="AG7" t="n">
-        <v>0.005030445523511956</v>
+        <v>0.004854814029621551</v>
       </c>
       <c r="AH7" t="n">
-        <v>0.005511559918566562</v>
+        <v>0.00531913093834206</v>
       </c>
       <c r="AI7" t="n">
-        <v>0.01375293812951665</v>
+        <v>0.01327277209694962</v>
       </c>
       <c r="AJ7" t="n">
-        <v>0.01380533206754999</v>
+        <v>0.01332333676845684</v>
       </c>
       <c r="AK7" t="n">
-        <v>0.03649159349982824</v>
+        <v>0.0352175367486199</v>
       </c>
       <c r="AL7" t="n">
-        <v>0.05768400022584465</v>
+        <v>0.05567003802589887</v>
       </c>
       <c r="AM7" t="n">
-        <v>0.01259195748465224</v>
+        <v>0.01215232558849169</v>
       </c>
       <c r="AN7" t="n">
-        <v>0.04709791485386385</v>
+        <v>0.0454535521217271</v>
       </c>
       <c r="AO7" t="n">
-        <v>0.02481856921577263</v>
+        <v>0.02395206099752134</v>
       </c>
       <c r="AP7" t="n">
-        <v>0.02285238472682107</v>
+        <v>0.02205452329491199</v>
       </c>
       <c r="AQ7" t="n">
-        <v>0.08373272890885505</v>
+        <v>0.08080930906521552</v>
       </c>
       <c r="AR7" t="n">
-        <v>16.61756327855648</v>
+        <v>15.9732912679159</v>
       </c>
       <c r="AS7" t="n">
-        <v>63.88352256053733</v>
+        <v>61.40672347531937</v>
       </c>
       <c r="AT7" t="n">
-        <v>0.168392062628633</v>
+        <v>0.1618634103258215</v>
       </c>
       <c r="AU7" t="n">
-        <v>0.5954886573407769</v>
+        <v>0.5724012366312872</v>
       </c>
       <c r="AV7" t="n">
-        <v>0.8581222823299828</v>
+        <v>0.8248524124372264</v>
       </c>
       <c r="AW7" t="n">
-        <v>0.06622542837339526</v>
+        <v>0.06365783231984394</v>
       </c>
       <c r="AX7" t="n">
-        <v>0.5534473477669504</v>
+        <v>0.5319898916073201</v>
       </c>
       <c r="AY7" t="n">
-        <v>0.7240319423984816</v>
+        <v>0.6959608282719587</v>
       </c>
       <c r="AZ7" t="n">
-        <v>0.9585735672412399</v>
+        <v>0.9214091461308138</v>
       </c>
       <c r="BA7" t="n">
-        <v>1.055657323654295</v>
+        <v>1.014728912246598</v>
       </c>
       <c r="BB7" t="n">
-        <v>0.01348110684445647</v>
+        <v>0.01295843696399654</v>
       </c>
       <c r="BC7" t="n">
-        <v>0.02045940003721293</v>
+        <v>0.01966617791568296</v>
       </c>
       <c r="BD7" t="n">
-        <v>0.02513569719726758</v>
+        <v>0.02416117247901159</v>
       </c>
       <c r="BE7" t="n">
-        <v>0.005301519530639837</v>
+        <v>0.005116726959194452</v>
       </c>
       <c r="BF7" t="n">
-        <v>0.002872100328802434</v>
+        <v>0.002771988879218756</v>
       </c>
       <c r="BG7" t="n">
-        <v>0.004622134473560608</v>
+        <v>0.004461022907339039</v>
       </c>
       <c r="BH7" t="n">
-        <v>0.002872100328802434</v>
+        <v>0.002771988879218756</v>
       </c>
       <c r="BI7" t="n">
-        <v>0.003160375760976735</v>
+        <v>0.00305021603031286</v>
       </c>
       <c r="BJ7" t="n">
-        <v>0.01334157846408812</v>
+        <v>0.01287653734195881</v>
       </c>
       <c r="BK7" t="n">
-        <v>0.01094288599551408</v>
+        <v>0.01056145496796476</v>
       </c>
       <c r="BL7" t="n">
-        <v>0.02043466727138483</v>
+        <v>0.01972238569062561</v>
       </c>
       <c r="BM7" t="n">
-        <v>0.0953317744264416</v>
+        <v>0.09200883962729595</v>
       </c>
       <c r="BN7" t="n">
-        <v>0.09497139153480001</v>
+        <v>0.09166101843251627</v>
       </c>
       <c r="BO7" t="n">
-        <v>0.153997291728012</v>
+        <v>0.1486294805996034</v>
       </c>
       <c r="BP7" t="n">
-        <v>0.165091495304421</v>
+        <v>0.1593369787427541</v>
       </c>
       <c r="BQ7" t="n">
-        <v>16.59505828405983</v>
+        <v>15.86830591351808</v>
       </c>
       <c r="BR7" t="n">
-        <v>65.01312568620331</v>
+        <v>62.16598635110614</v>
       </c>
     </row>
     <row r="8">
@@ -2214,211 +2214,211 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2767.506698541254</v>
+        <v>2658.246786635675</v>
       </c>
       <c r="C8" t="n">
-        <v>2572.618008845903</v>
+        <v>2471.052214204333</v>
       </c>
       <c r="D8" t="n">
-        <v>2992.042018529783</v>
+        <v>2873.917553814063</v>
       </c>
       <c r="E8" t="n">
-        <v>59.14973321294487</v>
+        <v>56.81452851642459</v>
       </c>
       <c r="F8" t="n">
-        <v>1226.664924540122</v>
+        <v>1178.236748498646</v>
       </c>
       <c r="G8" t="n">
-        <v>46.21124330285231</v>
+        <v>44.38684433211873</v>
       </c>
       <c r="H8" t="n">
-        <v>198.6853086875518</v>
+        <v>190.8413026240517</v>
       </c>
       <c r="I8" t="n">
-        <v>1118.464482917227</v>
+        <v>1074.308011340313</v>
       </c>
       <c r="J8" t="n">
-        <v>1114.086898028195</v>
+        <v>1070.103251521438</v>
       </c>
       <c r="K8" t="n">
-        <v>3864.897797712103</v>
+        <v>3712.313381882261</v>
       </c>
       <c r="L8" t="n">
-        <v>3925.576051742519</v>
+        <v>3770.596085906081</v>
       </c>
       <c r="M8" t="n">
-        <v>4080.790392934856</v>
+        <v>3919.682635156994</v>
       </c>
       <c r="N8" t="n">
-        <v>4226.45330739218</v>
+        <v>4059.594843677488</v>
       </c>
       <c r="O8" t="n">
-        <v>3999.154856918718</v>
+        <v>3841.27003315514</v>
       </c>
       <c r="P8" t="n">
-        <v>4150.507214741793</v>
+        <v>3986.647068392304</v>
       </c>
       <c r="Q8" t="n">
-        <v>3979.5889676867</v>
+        <v>3822.476596374627</v>
       </c>
       <c r="R8" t="n">
-        <v>3946.863812361923</v>
+        <v>3791.043415370911</v>
       </c>
       <c r="S8" t="n">
-        <v>3975.237437129783</v>
+        <v>3818.296862274627</v>
       </c>
       <c r="T8" t="n">
-        <v>3886.718529406019</v>
+        <v>3733.272640964801</v>
       </c>
       <c r="U8" t="n">
-        <v>4015.838771343871</v>
+        <v>3857.295274189803</v>
       </c>
       <c r="V8" t="n">
-        <v>3591.424315167376</v>
+        <v>3425.159587116713</v>
       </c>
       <c r="W8" t="n">
-        <v>3836.158038170043</v>
+        <v>3658.56338017264</v>
       </c>
       <c r="X8" t="n">
-        <v>3739.199634298526</v>
+        <v>3566.093658572344</v>
       </c>
       <c r="Y8" t="n">
-        <v>3576.613662439458</v>
+        <v>3411.034592482064</v>
       </c>
       <c r="Z8" t="n">
-        <v>3592.616065415773</v>
+        <v>3426.296165373842</v>
       </c>
       <c r="AA8" t="n">
-        <v>3340.141314767327</v>
+        <v>3185.509714985252</v>
       </c>
       <c r="AB8" t="n">
-        <v>3402.235140007568</v>
+        <v>3244.728911091977</v>
       </c>
       <c r="AC8" t="n">
-        <v>3596.029991261987</v>
+        <v>3429.552043770746</v>
       </c>
       <c r="AD8" t="n">
-        <v>3701.357177757523</v>
+        <v>3530.003115810781</v>
       </c>
       <c r="AE8" t="n">
-        <v>3679.298886265837</v>
+        <v>3508.966011322992</v>
       </c>
       <c r="AF8" t="n">
-        <v>3755.8319318406</v>
+        <v>3581.955965106668</v>
       </c>
       <c r="AG8" t="n">
-        <v>3672.564790204588</v>
+        <v>3508.97129165551</v>
       </c>
       <c r="AH8" t="n">
-        <v>2915.487715677523</v>
+        <v>2785.618029877378</v>
       </c>
       <c r="AI8" t="n">
-        <v>3827.2594675038</v>
+        <v>3656.775132465249</v>
       </c>
       <c r="AJ8" t="n">
-        <v>3244.94436654203</v>
+        <v>3100.399114968631</v>
       </c>
       <c r="AK8" t="n">
-        <v>3646.58076538238</v>
+        <v>3484.144718851137</v>
       </c>
       <c r="AL8" t="n">
-        <v>3649.806023073128</v>
+        <v>3487.226308228461</v>
       </c>
       <c r="AM8" t="n">
-        <v>3643.347995445457</v>
+        <v>3481.055951858804</v>
       </c>
       <c r="AN8" t="n">
-        <v>3722.748681382652</v>
+        <v>3556.919753699548</v>
       </c>
       <c r="AO8" t="n">
-        <v>3959.553461405854</v>
+        <v>3783.17612283005</v>
       </c>
       <c r="AP8" t="n">
-        <v>3725.992719688836</v>
+        <v>3560.019287114395</v>
       </c>
       <c r="AQ8" t="n">
-        <v>3192.071925927655</v>
+        <v>3049.881864264044</v>
       </c>
       <c r="AR8" t="n">
-        <v>2780.724280360283</v>
+        <v>2661.093667177803</v>
       </c>
       <c r="AS8" t="n">
-        <v>2532.138458622902</v>
+        <v>2423.202352081355</v>
       </c>
       <c r="AT8" t="n">
-        <v>3556.588640983284</v>
+        <v>3403.579267503241</v>
       </c>
       <c r="AU8" t="n">
-        <v>3699.262925249657</v>
+        <v>3540.11550628531</v>
       </c>
       <c r="AV8" t="n">
-        <v>3970.550869385049</v>
+        <v>3799.732267004515</v>
       </c>
       <c r="AW8" t="n">
-        <v>3807.53354535402</v>
+        <v>3643.728174227997</v>
       </c>
       <c r="AX8" t="n">
-        <v>3633.823079781073</v>
+        <v>3477.490973681531</v>
       </c>
       <c r="AY8" t="n">
-        <v>3809.677420622909</v>
+        <v>3645.779817010977</v>
       </c>
       <c r="AZ8" t="n">
-        <v>3887.743584644518</v>
+        <v>3720.48746644102</v>
       </c>
       <c r="BA8" t="n">
-        <v>4125.300541351408</v>
+        <v>3947.824393568809</v>
       </c>
       <c r="BB8" t="n">
-        <v>3478.910670055297</v>
+        <v>3329.243110561817</v>
       </c>
       <c r="BC8" t="n">
-        <v>3898.485916441172</v>
+        <v>3730.767648232757</v>
       </c>
       <c r="BD8" t="n">
-        <v>3704.434870616305</v>
+        <v>3545.064947392932</v>
       </c>
       <c r="BE8" t="n">
-        <v>3746.549524997754</v>
+        <v>3562.179727482458</v>
       </c>
       <c r="BF8" t="n">
-        <v>3696.361090022859</v>
+        <v>3514.461093462332</v>
       </c>
       <c r="BG8" t="n">
-        <v>3063.766770568619</v>
+        <v>2912.997094269153</v>
       </c>
       <c r="BH8" t="n">
-        <v>2704.013178363379</v>
+        <v>2570.947177541237</v>
       </c>
       <c r="BI8" t="n">
-        <v>3679.111111823214</v>
+        <v>3498.059996337552</v>
       </c>
       <c r="BJ8" t="n">
-        <v>3675.275333923229</v>
+        <v>3494.412979213319</v>
       </c>
       <c r="BK8" t="n">
-        <v>3725.981819361629</v>
+        <v>3542.624170143902</v>
       </c>
       <c r="BL8" t="n">
-        <v>1682.360919641895</v>
+        <v>1599.570997866549</v>
       </c>
       <c r="BM8" t="n">
-        <v>3286.808110984345</v>
+        <v>3125.062445579273</v>
       </c>
       <c r="BN8" t="n">
-        <v>3705.869704204047</v>
+        <v>3523.501783421635</v>
       </c>
       <c r="BO8" t="n">
-        <v>3487.086256880791</v>
+        <v>3315.484791903527</v>
       </c>
       <c r="BP8" t="n">
-        <v>3723.176427095911</v>
+        <v>3539.956832800594</v>
       </c>
       <c r="BQ8" t="n">
-        <v>2814.942636919459</v>
+        <v>2684.448641985472</v>
       </c>
       <c r="BR8" t="n">
-        <v>2569.610274391499</v>
+        <v>2450.489299871136</v>
       </c>
     </row>
     <row r="9">
@@ -2428,211 +2428,211 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>15.7463309971256</v>
+        <v>15.71980375411299</v>
       </c>
       <c r="C9" t="n">
-        <v>16.68791198449499</v>
+        <v>16.65979849592</v>
       </c>
       <c r="D9" t="n">
-        <v>1.060411110363846</v>
+        <v>1.058624676227346</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9544245343348747</v>
+        <v>0.9528166517389786</v>
       </c>
       <c r="F9" t="n">
-        <v>0.06761364447826407</v>
+        <v>0.0674997383512831</v>
       </c>
       <c r="G9" t="n">
-        <v>0.8943949406848504</v>
+        <v>0.8928881876548825</v>
       </c>
       <c r="H9" t="n">
-        <v>0.7867962656191698</v>
+        <v>0.7854707799715417</v>
       </c>
       <c r="I9" t="n">
-        <v>1.306553392404428</v>
+        <v>1.304352291757199</v>
       </c>
       <c r="J9" t="n">
-        <v>1.248154321780104</v>
+        <v>1.246051603818876</v>
       </c>
       <c r="K9" t="n">
-        <v>0.9453017119461095</v>
+        <v>0.9437091982210007</v>
       </c>
       <c r="L9" t="n">
-        <v>1.128518149267288</v>
+        <v>1.126616977801045</v>
       </c>
       <c r="M9" t="n">
-        <v>0.08248014543496177</v>
+        <v>0.08234119428106644</v>
       </c>
       <c r="N9" t="n">
-        <v>0.4662848150570075</v>
+        <v>0.4654992828206811</v>
       </c>
       <c r="O9" t="n">
-        <v>0.7964638853623976</v>
+        <v>0.7951221130446666</v>
       </c>
       <c r="P9" t="n">
-        <v>1.306378548748904</v>
+        <v>1.30417774265411</v>
       </c>
       <c r="Q9" t="n">
-        <v>1.253759636190715</v>
+        <v>1.251647475170176</v>
       </c>
       <c r="R9" t="n">
-        <v>0.1187649020734333</v>
+        <v>0.1185648233745132</v>
       </c>
       <c r="S9" t="n">
-        <v>0.5505417699902577</v>
+        <v>0.5496142932768704</v>
       </c>
       <c r="T9" t="n">
-        <v>-0.001869113683133161</v>
+        <v>-0.001865964858629236</v>
       </c>
       <c r="U9" t="n">
-        <v>-0.006600209816122458</v>
+        <v>-0.006589090694483364</v>
       </c>
       <c r="V9" t="n">
-        <v>0.007398119838755476</v>
+        <v>0.007277003735989391</v>
       </c>
       <c r="W9" t="n">
-        <v>0.08704639725937789</v>
+        <v>0.08562134324218616</v>
       </c>
       <c r="X9" t="n">
-        <v>-0.002254239667510583</v>
+        <v>-0.002217335058071934</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.01077279646380311</v>
+        <v>0.01059643285358514</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.304601980724113</v>
+        <v>0.2996152806429826</v>
       </c>
       <c r="AA9" t="n">
-        <v>1.486757938114067</v>
+        <v>1.462417925902098</v>
       </c>
       <c r="AB9" t="n">
-        <v>2.389900471954386</v>
+        <v>2.350774932294212</v>
       </c>
       <c r="AC9" t="n">
-        <v>2.79931105560014</v>
+        <v>2.753482973212475</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.01519492600347807</v>
+        <v>0.01494616682419044</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.2511489952925192</v>
+        <v>0.2470373847500541</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.01079284509245783</v>
+        <v>0.01061615326212159</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.02255230816740521</v>
+        <v>0.02200682653547766</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.02517599811208226</v>
+        <v>0.02456705624973967</v>
       </c>
       <c r="AI9" t="n">
-        <v>0.03952655693394461</v>
+        <v>0.03857051240755918</v>
       </c>
       <c r="AJ9" t="n">
-        <v>0.0114476207301989</v>
+        <v>0.01117073258237633</v>
       </c>
       <c r="AK9" t="n">
-        <v>0.062702945014516</v>
+        <v>0.06118632398755541</v>
       </c>
       <c r="AL9" t="n">
-        <v>0.120851107676054</v>
+        <v>0.1179280339513581</v>
       </c>
       <c r="AM9" t="n">
-        <v>0.1624737515971123</v>
+        <v>0.1585439344578327</v>
       </c>
       <c r="AN9" t="n">
-        <v>0.2953259712316627</v>
+        <v>0.2881828047077649</v>
       </c>
       <c r="AO9" t="n">
-        <v>0.4278872067031605</v>
+        <v>0.4175377289441301</v>
       </c>
       <c r="AP9" t="n">
-        <v>0.6219682932166206</v>
+        <v>0.6069244991591527</v>
       </c>
       <c r="AQ9" t="n">
-        <v>1.290666295816274</v>
+        <v>1.259448437666691</v>
       </c>
       <c r="AR9" t="n">
-        <v>16.16857599459583</v>
+        <v>15.53325581511781</v>
       </c>
       <c r="AS9" t="n">
-        <v>17.08894790316499</v>
+        <v>16.41746307651371</v>
       </c>
       <c r="AT9" t="n">
-        <v>0.2312725142137619</v>
+        <v>0.2221850042631188</v>
       </c>
       <c r="AU9" t="n">
-        <v>0.1798432960047457</v>
+        <v>0.1727766207988498</v>
       </c>
       <c r="AV9" t="n">
-        <v>0.1853598309251206</v>
+        <v>0.1780763916729117</v>
       </c>
       <c r="AW9" t="n">
-        <v>0.05467122524071794</v>
+        <v>0.05252300064482122</v>
       </c>
       <c r="AX9" t="n">
-        <v>0.02319250001474323</v>
+        <v>0.02228118517311244</v>
       </c>
       <c r="AY9" t="n">
-        <v>0.02553331493593515</v>
+        <v>0.02453002124865008</v>
       </c>
       <c r="AZ9" t="n">
-        <v>0.06621053416793636</v>
+        <v>0.06360888956639764</v>
       </c>
       <c r="BA9" t="n">
-        <v>0.07075110935887684</v>
+        <v>0.06797104959905789</v>
       </c>
       <c r="BB9" t="n">
-        <v>0.01478893117936625</v>
+        <v>0.01420782209379783</v>
       </c>
       <c r="BC9" t="n">
-        <v>0.1059971187541369</v>
+        <v>0.1018321194039443</v>
       </c>
       <c r="BD9" t="n">
-        <v>0.1161350540460953</v>
+        <v>0.1115716995858809</v>
       </c>
       <c r="BE9" t="n">
-        <v>0.001850943967399602</v>
+        <v>0.001773874488807443</v>
       </c>
       <c r="BF9" t="n">
-        <v>-0.001950554115279534</v>
+        <v>-0.0018693370761481</v>
       </c>
       <c r="BG9" t="n">
-        <v>-0.0007920221514355685</v>
+        <v>-0.0007590439871476804</v>
       </c>
       <c r="BH9" t="n">
-        <v>0.001615801545139479</v>
+        <v>0.001548522910677488</v>
       </c>
       <c r="BI9" t="n">
-        <v>-0.003197763405894659</v>
+        <v>-0.003064615151439595</v>
       </c>
       <c r="BJ9" t="n">
-        <v>0.04668835223975141</v>
+        <v>0.04474434581555916</v>
       </c>
       <c r="BK9" t="n">
-        <v>0.01042956426408363</v>
+        <v>0.009995298779048117</v>
       </c>
       <c r="BL9" t="n">
-        <v>0.008897754550954408</v>
+        <v>0.008527270454211882</v>
       </c>
       <c r="BM9" t="n">
-        <v>0.002432292391437542</v>
+        <v>0.002331016766840907</v>
       </c>
       <c r="BN9" t="n">
-        <v>6.819997929758624e-05</v>
+        <v>6.53602732140761e-05</v>
       </c>
       <c r="BO9" t="n">
-        <v>0.1146412150729097</v>
+        <v>0.109867791983688</v>
       </c>
       <c r="BP9" t="n">
-        <v>0.06642868874112089</v>
+        <v>0.06366273553291457</v>
       </c>
       <c r="BQ9" t="n">
-        <v>16.10231039294852</v>
+        <v>15.4078086730526</v>
       </c>
       <c r="BR9" t="n">
-        <v>17.18981820088023</v>
+        <v>16.44841165648537</v>
       </c>
     </row>
     <row r="10">
@@ -2642,211 +2642,211 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2611.374707882053</v>
+        <v>2602.541778645161</v>
       </c>
       <c r="C10" t="n">
-        <v>2757.516657313795</v>
+        <v>2748.189405491188</v>
       </c>
       <c r="D10" t="n">
-        <v>2899.260189887431</v>
+        <v>2889.453493047137</v>
       </c>
       <c r="E10" t="n">
-        <v>40.83515065893477</v>
+        <v>40.69702647665657</v>
       </c>
       <c r="F10" t="n">
-        <v>1200.743946066561</v>
+        <v>1196.6824506882</v>
       </c>
       <c r="G10" t="n">
-        <v>29.849649623698</v>
+        <v>29.74868370636858</v>
       </c>
       <c r="H10" t="n">
-        <v>187.4020732633952</v>
+        <v>186.7681890310841</v>
       </c>
       <c r="I10" t="n">
-        <v>1074.473098628611</v>
+        <v>1070.838712181318</v>
       </c>
       <c r="J10" t="n">
-        <v>1082.883240045366</v>
+        <v>1079.220406441951</v>
       </c>
       <c r="K10" t="n">
-        <v>3667.071315574016</v>
+        <v>3654.667511041739</v>
       </c>
       <c r="L10" t="n">
-        <v>3659.185455682351</v>
+        <v>3646.808324933114</v>
       </c>
       <c r="M10" t="n">
-        <v>3868.333284138774</v>
+        <v>3855.248714520949</v>
       </c>
       <c r="N10" t="n">
-        <v>3959.910009702146</v>
+        <v>3946.515683413167</v>
       </c>
       <c r="O10" t="n">
-        <v>3811.133892353869</v>
+        <v>3798.242798677471</v>
       </c>
       <c r="P10" t="n">
-        <v>3868.329400571922</v>
+        <v>3855.244844090193</v>
       </c>
       <c r="Q10" t="n">
-        <v>3782.086476682847</v>
+        <v>3769.293635381478</v>
       </c>
       <c r="R10" t="n">
-        <v>3675.878135604992</v>
+        <v>3663.444542158125</v>
       </c>
       <c r="S10" t="n">
-        <v>3682.707110517507</v>
+        <v>3670.250418182541</v>
       </c>
       <c r="T10" t="n">
-        <v>3732.978219037525</v>
+        <v>3720.351485557994</v>
       </c>
       <c r="U10" t="n">
-        <v>3687.534384115184</v>
+        <v>3675.061363611776</v>
       </c>
       <c r="V10" t="n">
-        <v>3499.245001193692</v>
+        <v>3451.692813224554</v>
       </c>
       <c r="W10" t="n">
-        <v>3660.957261795576</v>
+        <v>3611.207522123018</v>
       </c>
       <c r="X10" t="n">
-        <v>3544.166184033897</v>
+        <v>3496.003549945815</v>
       </c>
       <c r="Y10" t="n">
-        <v>3401.138076260048</v>
+        <v>3354.919089862657</v>
       </c>
       <c r="Z10" t="n">
-        <v>3447.281164086586</v>
+        <v>3400.435126772481</v>
       </c>
       <c r="AA10" t="n">
-        <v>3251.203548998231</v>
+        <v>3207.022063496314</v>
       </c>
       <c r="AB10" t="n">
-        <v>3238.457970124436</v>
+        <v>3194.449687745529</v>
       </c>
       <c r="AC10" t="n">
-        <v>3472.500904282328</v>
+        <v>3425.31214908882</v>
       </c>
       <c r="AD10" t="n">
-        <v>3501.993892910685</v>
+        <v>3454.404349507563</v>
       </c>
       <c r="AE10" t="n">
-        <v>3449.437776417178</v>
+        <v>3402.562432314069</v>
       </c>
       <c r="AF10" t="n">
-        <v>3593.446353796935</v>
+        <v>3544.614038136136</v>
       </c>
       <c r="AG10" t="n">
-        <v>3563.735190968476</v>
+        <v>3496.180139878022</v>
       </c>
       <c r="AH10" t="n">
-        <v>2852.843030487208</v>
+        <v>2798.763828091354</v>
       </c>
       <c r="AI10" t="n">
-        <v>3692.731617150276</v>
+        <v>3622.731277705266</v>
       </c>
       <c r="AJ10" t="n">
-        <v>3139.775525467885</v>
+        <v>3080.257159296043</v>
       </c>
       <c r="AK10" t="n">
-        <v>3536.243179294975</v>
+        <v>3469.209273618997</v>
       </c>
       <c r="AL10" t="n">
-        <v>3500.622322799913</v>
+        <v>3434.263654943657</v>
       </c>
       <c r="AM10" t="n">
-        <v>3427.832283131885</v>
+        <v>3362.853441380865</v>
       </c>
       <c r="AN10" t="n">
-        <v>3597.59335306254</v>
+        <v>3529.396478226065</v>
       </c>
       <c r="AO10" t="n">
-        <v>3781.174653005251</v>
+        <v>3709.497765364146</v>
       </c>
       <c r="AP10" t="n">
-        <v>3554.842304286414</v>
+        <v>3487.455828968837</v>
       </c>
       <c r="AQ10" t="n">
-        <v>3110.106617352163</v>
+        <v>3051.150662385462</v>
       </c>
       <c r="AR10" t="n">
-        <v>2665.70714710587</v>
+        <v>2606.849499539889</v>
       </c>
       <c r="AS10" t="n">
-        <v>2757.198078149534</v>
+        <v>2696.320350853229</v>
       </c>
       <c r="AT10" t="n">
-        <v>3391.736903200387</v>
+        <v>3316.848836256561</v>
       </c>
       <c r="AU10" t="n">
-        <v>3495.893361574008</v>
+        <v>3418.705565597558</v>
       </c>
       <c r="AV10" t="n">
-        <v>3729.050177381914</v>
+        <v>3646.714380918115</v>
       </c>
       <c r="AW10" t="n">
-        <v>3609.994531430692</v>
+        <v>3530.287431542863</v>
       </c>
       <c r="AX10" t="n">
-        <v>3440.699150429205</v>
+        <v>3364.730018487463</v>
       </c>
       <c r="AY10" t="n">
-        <v>3710.259964017934</v>
+        <v>3628.339047244527</v>
       </c>
       <c r="AZ10" t="n">
-        <v>3679.648971863129</v>
+        <v>3598.403932404246</v>
       </c>
       <c r="BA10" t="n">
-        <v>3883.508042631663</v>
+        <v>3797.761884078191</v>
       </c>
       <c r="BB10" t="n">
-        <v>3291.364192731181</v>
+        <v>3218.692311321633</v>
       </c>
       <c r="BC10" t="n">
-        <v>3694.157398460051</v>
+        <v>3612.592019289319</v>
       </c>
       <c r="BD10" t="n">
-        <v>3504.8062360378</v>
+        <v>3427.421647692556</v>
       </c>
       <c r="BE10" t="n">
-        <v>3630.64846357072</v>
+        <v>3534.511578962228</v>
       </c>
       <c r="BF10" t="n">
-        <v>3566.04928714053</v>
+        <v>3471.622940920039</v>
       </c>
       <c r="BG10" t="n">
-        <v>2928.660228624924</v>
+        <v>2851.111473001283</v>
       </c>
       <c r="BH10" t="n">
-        <v>2590.235768668259</v>
+        <v>2521.648242307653</v>
       </c>
       <c r="BI10" t="n">
-        <v>3562.670682284719</v>
+        <v>3468.333799020616</v>
       </c>
       <c r="BJ10" t="n">
-        <v>3563.826934582566</v>
+        <v>3469.459434613252</v>
       </c>
       <c r="BK10" t="n">
-        <v>3570.74400691923</v>
+        <v>3476.193347993126</v>
       </c>
       <c r="BL10" t="n">
-        <v>1617.806620589094</v>
+        <v>1574.968298464825</v>
       </c>
       <c r="BM10" t="n">
-        <v>3177.049534018038</v>
+        <v>3092.92361339752</v>
       </c>
       <c r="BN10" t="n">
-        <v>3566.966531710444</v>
+        <v>3472.515897532509</v>
       </c>
       <c r="BO10" t="n">
-        <v>3346.126011800022</v>
+        <v>3257.523071165689</v>
       </c>
       <c r="BP10" t="n">
-        <v>3596.70779378511</v>
+        <v>3501.469632996193</v>
       </c>
       <c r="BQ10" t="n">
-        <v>2707.906608336544</v>
+        <v>2638.484135996975</v>
       </c>
       <c r="BR10" t="n">
-        <v>2801.073537307837</v>
+        <v>2729.262548861559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
plus besoin excel 2
</commit_message>
<xml_diff>
--- a/data/concentration_corrigeelin.xlsx
+++ b/data/concentration_corrigeelin.xlsx
@@ -1358,97 +1358,97 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>16.56963241710433</v>
+        <v>15.85673476965436</v>
       </c>
       <c r="C4" t="n">
-        <v>2972.211151210834</v>
+        <v>2844.333701422901</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2447301933450663</v>
+        <v>0.2342008361026222</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3706929487371821</v>
+        <v>0.3547441259492827</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3383077500961947</v>
+        <v>0.3237522793961501</v>
       </c>
       <c r="G4" t="n">
-        <v>0.433598073139414</v>
+        <v>0.4149427983271107</v>
       </c>
       <c r="H4" t="n">
-        <v>0.8577642003963535</v>
+        <v>0.8208594541028789</v>
       </c>
       <c r="I4" t="n">
-        <v>0.6694986609442172</v>
+        <v>0.6406939169195186</v>
       </c>
       <c r="J4" t="n">
-        <v>0.736573647164795</v>
+        <v>0.7048830455256553</v>
       </c>
       <c r="K4" t="n">
-        <v>0.4546532863508104</v>
+        <v>0.4350921246976218</v>
       </c>
       <c r="L4" t="n">
-        <v>0.332883450802229</v>
+        <v>0.3185613570479362</v>
       </c>
       <c r="M4" t="n">
-        <v>0.4131953615881837</v>
+        <v>0.3954179001576341</v>
       </c>
       <c r="N4" t="n">
-        <v>0.8821571638855118</v>
+        <v>0.8442029262184203</v>
       </c>
       <c r="O4" t="n">
-        <v>0.8867691734500209</v>
+        <v>0.8486165070739641</v>
       </c>
       <c r="P4" t="n">
-        <v>0.7634686086503123</v>
+        <v>0.7306208688026333</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.749854665146761</v>
+        <v>0.7175926563552628</v>
       </c>
       <c r="R4" t="n">
-        <v>0.4135998883458812</v>
+        <v>0.3958050224149399</v>
       </c>
       <c r="S4" t="n">
-        <v>0.6378331154051736</v>
+        <v>0.6103907608621331</v>
       </c>
       <c r="T4" t="n">
-        <v>0.3379857467970674</v>
+        <v>0.3234441300793346</v>
       </c>
       <c r="U4" t="n">
-        <v>0.1595012598192988</v>
+        <v>0.152638821955372</v>
       </c>
       <c r="V4" t="n">
-        <v>0.1269360380684472</v>
+        <v>0.1222119178755813</v>
       </c>
       <c r="W4" t="n">
-        <v>0.1536378578467219</v>
+        <v>0.147919988298509</v>
       </c>
       <c r="X4" t="n">
-        <v>0.05081743437212209</v>
+        <v>0.04892618527123609</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.1776091677145319</v>
+        <v>0.1709991689434509</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.01439702191252692</v>
+        <v>0.0138612145644401</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.03291859184365315</v>
+        <v>0.03169347573938765</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.1186091497261071</v>
+        <v>0.1141949275098944</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.1448376033275961</v>
+        <v>0.1394472488074933</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.2466564508734998</v>
+        <v>0.2374767510971146</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.2371599552233581</v>
+        <v>0.2283336821612848</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.4653765180861303</v>
+        <v>0.4480568140853575</v>
       </c>
       <c r="AG4" t="n">
         <v>-0.02063148376841588</v>
@@ -1484,85 +1484,85 @@
         <v>17.35246083407053</v>
       </c>
       <c r="AR4" t="n">
-        <v>16.43590608149136</v>
+        <v>15.68477249500009</v>
       </c>
       <c r="AS4" t="n">
-        <v>3004.348389465385</v>
+        <v>2867.047350529075</v>
       </c>
       <c r="AT4" t="n">
-        <v>3.252546101212474</v>
+        <v>3.103902235390978</v>
       </c>
       <c r="AU4" t="n">
-        <v>2.878405904291459</v>
+        <v>2.746860534078934</v>
       </c>
       <c r="AV4" t="n">
-        <v>3.321915011016567</v>
+        <v>3.170100932506231</v>
       </c>
       <c r="AW4" t="n">
-        <v>2.419447491966248</v>
+        <v>2.308876875234968</v>
       </c>
       <c r="AX4" t="n">
-        <v>0.9646065702504453</v>
+        <v>0.9205233058978229</v>
       </c>
       <c r="AY4" t="n">
-        <v>1.044029714073639</v>
+        <v>0.9963167507817223</v>
       </c>
       <c r="AZ4" t="n">
-        <v>0.7639143747446607</v>
+        <v>0.7290028985395032</v>
       </c>
       <c r="BA4" t="n">
-        <v>0.6827621435856952</v>
+        <v>0.651559386944885</v>
       </c>
       <c r="BB4" t="n">
-        <v>3.853085854164722</v>
+        <v>3.676996858380262</v>
       </c>
       <c r="BC4" t="n">
-        <v>0.6929835027705826</v>
+        <v>0.6613136221303231</v>
       </c>
       <c r="BD4" t="n">
-        <v>1.114838532824015</v>
+        <v>1.063889551893675</v>
       </c>
       <c r="BE4" t="n">
-        <v>0.994971917106736</v>
+        <v>0.9459959602198982</v>
       </c>
       <c r="BF4" t="n">
-        <v>1.358941272998196</v>
+        <v>1.292049486351956</v>
       </c>
       <c r="BG4" t="n">
-        <v>1.228803695157168</v>
+        <v>1.16831772991364</v>
       </c>
       <c r="BH4" t="n">
-        <v>1.756225783608048</v>
+        <v>1.66977828013312</v>
       </c>
       <c r="BI4" t="n">
-        <v>1.89856868400293</v>
+        <v>1.805114570961413</v>
       </c>
       <c r="BJ4" t="n">
-        <v>2.410957013409261</v>
+        <v>2.292281375720801</v>
       </c>
       <c r="BK4" t="n">
-        <v>2.541666721809817</v>
+        <v>2.416557100474932</v>
       </c>
       <c r="BL4" t="n">
-        <v>0.9857130281196268</v>
+        <v>0.937192825752144</v>
       </c>
       <c r="BM4" t="n">
-        <v>-0.01685689149916791</v>
+        <v>-0.01602713703362475</v>
       </c>
       <c r="BN4" t="n">
-        <v>0.0715438784687218</v>
+        <v>0.06802224147861428</v>
       </c>
       <c r="BO4" t="n">
-        <v>0.04614229081116487</v>
+        <v>0.04387100776631375</v>
       </c>
       <c r="BP4" t="n">
-        <v>-0.1330475254697844</v>
+        <v>-0.1264984663865323</v>
       </c>
       <c r="BQ4" t="n">
-        <v>16.97999846527934</v>
+        <v>16.11778401744839</v>
       </c>
       <c r="BR4" t="n">
-        <v>3070.948728483208</v>
+        <v>2915.011355010498</v>
       </c>
     </row>
     <row r="5">

</xml_diff>